<commit_message>
Redo all with better monad
</commit_message>
<xml_diff>
--- a/app/librariandb.xlsx
+++ b/app/librariandb.xlsx
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Ntres</t>
+  </si>
+  <si>
+    <t>Pescador</t>
+  </si>
+  <si>
+    <t>Pipo</t>
   </si>
   <si>
     <t>Texto</t>
@@ -164,7 +170,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" t="n">
         <v>10</v>
@@ -215,6 +221,17 @@
       </c>
       <c r="C6" s="0" t="n">
         <v>505</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" outlineLevel="0" r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="n">
+        <v>666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed crea and other bugs
</commit_message>
<xml_diff>
--- a/app/librariandb.xlsx
+++ b/app/librariandb.xlsx
@@ -5,7 +5,9 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Alumnos" sheetId="1" r:id="rId3"/>
+    <sheet name="Librarian" sheetId="2" r:id="rId4"/>
+    <sheet name="Personas" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames/>
 </workbook>
@@ -15,46 +17,55 @@
 <!--Shared string table generated by xlsx-->
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Acinco</t>
-  </si>
-  <si>
-    <t>Acuatro</t>
-  </si>
-  <si>
-    <t>Ados</t>
-  </si>
-  <si>
     <t>Apellido</t>
   </si>
   <si>
-    <t>Atres</t>
-  </si>
-  <si>
     <t>DNI</t>
   </si>
   <si>
-    <t>Ncinco</t>
-  </si>
-  <si>
-    <t>Ncuatro</t>
-  </si>
-  <si>
-    <t>Ndos</t>
+    <t>Debe_libros</t>
+  </si>
+  <si>
+    <t>Dias_retraso</t>
+  </si>
+  <si>
+    <t>Errante</t>
+  </si>
+  <si>
+    <t>Holandes</t>
+  </si>
+  <si>
+    <t>Lucifer</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Marcos</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
   </si>
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Ntres</t>
-  </si>
-  <si>
     <t>Pescador</t>
   </si>
   <si>
+    <t>Peña</t>
+  </si>
+  <si>
     <t>Pipo</t>
   </si>
   <si>
-    <t>Texto</t>
+    <t>Polo</t>
+  </si>
+  <si>
+    <t>Soncini</t>
   </si>
 </sst>
 </file>
@@ -129,7 +140,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -154,87 +173,217 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col customWidth="1" max="1025" min="1" width="9.44897959183673"/>
+    <col customWidth="1" max="1025" min="1" width="9.31632653061224"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>221</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>666</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>667</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C7" activeCellId="0" pane="topLeft" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="8.23469387755102"/>
+    <col customWidth="1" max="2" min="2" width="11.9438775510204"/>
+    <col customWidth="1" max="3" min="3" width="15.8367346938776"/>
+    <col customWidth="1" max="1025" min="4" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+        <f>TRUE()</f>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+        <f>TRUE()</f>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="n">
-        <v>10</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>101</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>202</v>
-      </c>
-    </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>4</v>
+      <c r="A4" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>0</v>
+        <f>FALSE()</f>
       </c>
       <c r="C4" s="0" t="n">
-        <v>303</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>1</v>
+      <c r="A5" s="0" t="n">
+        <v>666</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>1</v>
+        <f>TRUE()</f>
       </c>
       <c r="C5" s="0" t="n">
-        <v>404</v>
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>0</v>
+      <c r="A6" s="0" t="n">
+        <v>667</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+        <f>FALSE()</f>
       </c>
       <c r="C6" s="0" t="n">
-        <v>505</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" outlineLevel="0" r="7">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="n">
-        <v>666</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetData>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" outlineLevel="0" r="1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" outlineLevel="0" r="2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" outlineLevel="0" r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>